<commit_message>
Master user belum fix
</commit_message>
<xml_diff>
--- a/public/master_gedung.xlsx
+++ b/public/master_gedung.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
   <si>
     <t>No.</t>
   </si>
@@ -132,6 +132,24 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>Gedung Lab Fisika</t>
+  </si>
+  <si>
+    <t>Hak A</t>
+  </si>
+  <si>
+    <t>Khusus</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
   </si>
 </sst>
 </file>
@@ -482,7 +500,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="I18" sqref="I18"/>
@@ -1062,6 +1080,68 @@
         <v>38</v>
       </c>
     </row>
+    <row r="10" spans="1:20">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10">
+        <v>67.8</v>
+      </c>
+      <c r="D10">
+        <v>89.8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10">
+        <v>1714.98</v>
+      </c>
+      <c r="I10">
+        <v>7</v>
+      </c>
+      <c r="J10">
+        <v>9000.0</v>
+      </c>
+      <c r="K10">
+        <v>899.0</v>
+      </c>
+      <c r="L10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" t="s">
+        <v>41</v>
+      </c>
+      <c r="N10" t="s">
+        <v>25</v>
+      </c>
+      <c r="O10" t="s">
+        <v>26</v>
+      </c>
+      <c r="P10" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" t="s">
+        <v>42</v>
+      </c>
+      <c r="S10" t="s">
+        <v>43</v>
+      </c>
+      <c r="T10" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>

<commit_message>
Perbaikan master jenis gedung
</commit_message>
<xml_diff>
--- a/public/master_gedung.xlsx
+++ b/public/master_gedung.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <t>No.</t>
   </si>
@@ -119,37 +119,34 @@
     <t>SDN Semboro 1</t>
   </si>
   <si>
+    <t>SDN Semboro 21</t>
+  </si>
+  <si>
+    <t>Universitas Jember</t>
+  </si>
+  <si>
+    <t>Tinggi</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Gedung Lab Biologi</t>
+  </si>
+  <si>
+    <t>Hak A</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
     <t>SDN Pondok Dalem 1</t>
-  </si>
-  <si>
-    <t>SDN Semboro 21</t>
-  </si>
-  <si>
-    <t>Universitas Jember</t>
-  </si>
-  <si>
-    <t>Tinggi</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Gedung Lab Fisika</t>
-  </si>
-  <si>
-    <t>Hak A</t>
-  </si>
-  <si>
-    <t>Khusus</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>k</t>
   </si>
 </sst>
 </file>
@@ -500,7 +497,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="I18" sqref="I18"/>
@@ -964,10 +961,10 @@
         <v>35</v>
       </c>
       <c r="C8">
-        <v>1.0</v>
+        <v>113.22</v>
       </c>
       <c r="D8">
-        <v>1.0</v>
+        <v>8.11</v>
       </c>
       <c r="E8" t="s">
         <v>21</v>
@@ -979,19 +976,19 @@
         <v>23</v>
       </c>
       <c r="H8">
-        <v>1.0</v>
+        <v>300.2</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J8">
-        <v>1.0</v>
+        <v>297.3</v>
       </c>
       <c r="K8">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="L8" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="M8" t="s">
         <v>24</v>
@@ -1009,13 +1006,13 @@
         <v>28</v>
       </c>
       <c r="R8" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="S8" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="T8" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -1023,37 +1020,37 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C9">
-        <v>113.22</v>
+        <v>67.8</v>
       </c>
       <c r="D9">
-        <v>8.11</v>
+        <v>89.8</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="H9">
-        <v>300.2</v>
+        <v>1714.98</v>
       </c>
       <c r="I9">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J9">
-        <v>297.3</v>
+        <v>9000.0</v>
       </c>
       <c r="K9">
-        <v>10.0</v>
+        <v>899.0</v>
       </c>
       <c r="L9" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="M9" t="s">
         <v>24</v>
@@ -1071,13 +1068,13 @@
         <v>28</v>
       </c>
       <c r="R9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="S9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="T9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -1085,61 +1082,1487 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C10">
-        <v>67.8</v>
+        <v>121.2</v>
       </c>
       <c r="D10">
-        <v>89.8</v>
+        <v>12.33</v>
       </c>
       <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10">
+        <v>123.12</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>112.314</v>
+      </c>
+      <c r="K10">
+        <v>11.0</v>
+      </c>
+      <c r="L10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" t="s">
+        <v>24</v>
+      </c>
+      <c r="N10" t="s">
+        <v>25</v>
+      </c>
+      <c r="O10" t="s">
+        <v>26</v>
+      </c>
+      <c r="P10" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" t="s">
+        <v>29</v>
+      </c>
+      <c r="S10" t="s">
+        <v>29</v>
+      </c>
+      <c r="T10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>113.0</v>
+      </c>
+      <c r="D11">
+        <v>8.0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11">
+        <v>50.0</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>45.0</v>
+      </c>
+      <c r="K11">
+        <v>10.0</v>
+      </c>
+      <c r="L11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" t="s">
+        <v>25</v>
+      </c>
+      <c r="O11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>28</v>
+      </c>
+      <c r="R11" t="s">
+        <v>29</v>
+      </c>
+      <c r="S11" t="s">
+        <v>29</v>
+      </c>
+      <c r="T11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12">
+        <v>113.567</v>
+      </c>
+      <c r="D12">
+        <v>8.768</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12">
+        <v>129.2</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>110.2</v>
+      </c>
+      <c r="K12">
+        <v>10.66</v>
+      </c>
+      <c r="L12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M12" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" t="s">
+        <v>25</v>
+      </c>
+      <c r="O12" t="s">
+        <v>26</v>
+      </c>
+      <c r="P12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>28</v>
+      </c>
+      <c r="R12" t="s">
+        <v>29</v>
+      </c>
+      <c r="S12" t="s">
+        <v>29</v>
+      </c>
+      <c r="T12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <v>121.13</v>
+      </c>
+      <c r="D13">
+        <v>11.2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13">
+        <v>312.1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>12.3</v>
+      </c>
+      <c r="K13">
+        <v>12.0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" t="s">
+        <v>25</v>
+      </c>
+      <c r="O13" t="s">
+        <v>26</v>
+      </c>
+      <c r="P13" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>28</v>
+      </c>
+      <c r="R13" t="s">
+        <v>29</v>
+      </c>
+      <c r="S13" t="s">
+        <v>29</v>
+      </c>
+      <c r="T13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14">
+        <v>1.0</v>
+      </c>
+      <c r="D14">
+        <v>1.0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14">
+        <v>1.0</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1.0</v>
+      </c>
+      <c r="K14">
+        <v>1.0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" t="s">
+        <v>25</v>
+      </c>
+      <c r="O14" t="s">
+        <v>26</v>
+      </c>
+      <c r="P14" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>28</v>
+      </c>
+      <c r="R14" t="s">
+        <v>29</v>
+      </c>
+      <c r="S14" t="s">
+        <v>29</v>
+      </c>
+      <c r="T14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15">
+        <v>1.0</v>
+      </c>
+      <c r="D15">
+        <v>1.0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15">
+        <v>1.0</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1.0</v>
+      </c>
+      <c r="K15">
+        <v>1.0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>24</v>
+      </c>
+      <c r="M15" t="s">
+        <v>24</v>
+      </c>
+      <c r="N15" t="s">
+        <v>25</v>
+      </c>
+      <c r="O15" t="s">
+        <v>26</v>
+      </c>
+      <c r="P15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>28</v>
+      </c>
+      <c r="R15" t="s">
+        <v>29</v>
+      </c>
+      <c r="S15" t="s">
+        <v>29</v>
+      </c>
+      <c r="T15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16">
+        <v>1.0</v>
+      </c>
+      <c r="D16">
+        <v>1.0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16">
+        <v>1.0</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1.0</v>
+      </c>
+      <c r="K16">
+        <v>1.0</v>
+      </c>
+      <c r="L16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M16" t="s">
+        <v>24</v>
+      </c>
+      <c r="N16" t="s">
+        <v>25</v>
+      </c>
+      <c r="O16" t="s">
+        <v>26</v>
+      </c>
+      <c r="P16" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>28</v>
+      </c>
+      <c r="R16" t="s">
+        <v>29</v>
+      </c>
+      <c r="S16" t="s">
+        <v>29</v>
+      </c>
+      <c r="T16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17">
+        <v>113.22</v>
+      </c>
+      <c r="D17">
+        <v>8.11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17">
+        <v>300.2</v>
+      </c>
+      <c r="I17">
         <v>4</v>
       </c>
-      <c r="F10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10">
-        <v>1714.98</v>
-      </c>
-      <c r="I10">
-        <v>7</v>
-      </c>
-      <c r="J10">
-        <v>9000.0</v>
-      </c>
-      <c r="K10">
-        <v>899.0</v>
-      </c>
-      <c r="L10" t="s">
-        <v>24</v>
-      </c>
-      <c r="M10" t="s">
-        <v>41</v>
-      </c>
-      <c r="N10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O10" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>28</v>
-      </c>
-      <c r="R10" t="s">
-        <v>42</v>
-      </c>
-      <c r="S10" t="s">
+      <c r="J17">
+        <v>297.3</v>
+      </c>
+      <c r="K17">
+        <v>10.0</v>
+      </c>
+      <c r="L17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" t="s">
+        <v>24</v>
+      </c>
+      <c r="N17" t="s">
+        <v>25</v>
+      </c>
+      <c r="O17" t="s">
+        <v>26</v>
+      </c>
+      <c r="P17" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>28</v>
+      </c>
+      <c r="R17" t="s">
+        <v>37</v>
+      </c>
+      <c r="S17" t="s">
+        <v>37</v>
+      </c>
+      <c r="T17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>121.2</v>
+      </c>
+      <c r="D18">
+        <v>12.33</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18">
+        <v>123.12</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>112.314</v>
+      </c>
+      <c r="K18">
+        <v>11.0</v>
+      </c>
+      <c r="L18" t="s">
+        <v>24</v>
+      </c>
+      <c r="M18" t="s">
+        <v>24</v>
+      </c>
+      <c r="N18" t="s">
+        <v>25</v>
+      </c>
+      <c r="O18" t="s">
+        <v>26</v>
+      </c>
+      <c r="P18" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>28</v>
+      </c>
+      <c r="R18" t="s">
+        <v>29</v>
+      </c>
+      <c r="S18" t="s">
+        <v>29</v>
+      </c>
+      <c r="T18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <v>113.0</v>
+      </c>
+      <c r="D19">
+        <v>8.0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19">
+        <v>50.0</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="J19">
+        <v>45.0</v>
+      </c>
+      <c r="K19">
+        <v>10.0</v>
+      </c>
+      <c r="L19" t="s">
+        <v>24</v>
+      </c>
+      <c r="M19" t="s">
+        <v>24</v>
+      </c>
+      <c r="N19" t="s">
+        <v>25</v>
+      </c>
+      <c r="O19" t="s">
+        <v>26</v>
+      </c>
+      <c r="P19" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>28</v>
+      </c>
+      <c r="R19" t="s">
+        <v>29</v>
+      </c>
+      <c r="S19" t="s">
+        <v>29</v>
+      </c>
+      <c r="T19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20">
+        <v>113.567</v>
+      </c>
+      <c r="D20">
+        <v>8.768</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20">
+        <v>129.2</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <v>110.2</v>
+      </c>
+      <c r="K20">
+        <v>10.66</v>
+      </c>
+      <c r="L20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M20" t="s">
+        <v>24</v>
+      </c>
+      <c r="N20" t="s">
+        <v>25</v>
+      </c>
+      <c r="O20" t="s">
+        <v>26</v>
+      </c>
+      <c r="P20" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>28</v>
+      </c>
+      <c r="R20" t="s">
+        <v>29</v>
+      </c>
+      <c r="S20" t="s">
+        <v>29</v>
+      </c>
+      <c r="T20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21">
+        <v>121.13</v>
+      </c>
+      <c r="D21">
+        <v>11.2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21">
+        <v>312.1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>12.3</v>
+      </c>
+      <c r="K21">
+        <v>12.0</v>
+      </c>
+      <c r="L21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M21" t="s">
+        <v>24</v>
+      </c>
+      <c r="N21" t="s">
+        <v>25</v>
+      </c>
+      <c r="O21" t="s">
+        <v>26</v>
+      </c>
+      <c r="P21" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>28</v>
+      </c>
+      <c r="R21" t="s">
+        <v>29</v>
+      </c>
+      <c r="S21" t="s">
+        <v>29</v>
+      </c>
+      <c r="T21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22">
+        <v>1.0</v>
+      </c>
+      <c r="D22">
+        <v>1.0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22">
+        <v>1.0</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1.0</v>
+      </c>
+      <c r="K22">
+        <v>1.0</v>
+      </c>
+      <c r="L22" t="s">
+        <v>24</v>
+      </c>
+      <c r="M22" t="s">
+        <v>24</v>
+      </c>
+      <c r="N22" t="s">
+        <v>25</v>
+      </c>
+      <c r="O22" t="s">
+        <v>26</v>
+      </c>
+      <c r="P22" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>28</v>
+      </c>
+      <c r="R22" t="s">
+        <v>29</v>
+      </c>
+      <c r="S22" t="s">
+        <v>29</v>
+      </c>
+      <c r="T22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>43</v>
       </c>
-      <c r="T10" t="s">
-        <v>44</v>
+      <c r="C23">
+        <v>1.0</v>
+      </c>
+      <c r="D23">
+        <v>1.0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23">
+        <v>1.0</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>1.0</v>
+      </c>
+      <c r="K23">
+        <v>1.0</v>
+      </c>
+      <c r="L23" t="s">
+        <v>24</v>
+      </c>
+      <c r="M23" t="s">
+        <v>24</v>
+      </c>
+      <c r="N23" t="s">
+        <v>25</v>
+      </c>
+      <c r="O23" t="s">
+        <v>26</v>
+      </c>
+      <c r="P23" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>28</v>
+      </c>
+      <c r="R23" t="s">
+        <v>29</v>
+      </c>
+      <c r="S23" t="s">
+        <v>29</v>
+      </c>
+      <c r="T23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24">
+        <v>1.0</v>
+      </c>
+      <c r="D24">
+        <v>1.0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24">
+        <v>1.0</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1.0</v>
+      </c>
+      <c r="K24">
+        <v>1.0</v>
+      </c>
+      <c r="L24" t="s">
+        <v>24</v>
+      </c>
+      <c r="M24" t="s">
+        <v>24</v>
+      </c>
+      <c r="N24" t="s">
+        <v>25</v>
+      </c>
+      <c r="O24" t="s">
+        <v>26</v>
+      </c>
+      <c r="P24" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>28</v>
+      </c>
+      <c r="R24" t="s">
+        <v>29</v>
+      </c>
+      <c r="S24" t="s">
+        <v>29</v>
+      </c>
+      <c r="T24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25">
+        <v>113.22</v>
+      </c>
+      <c r="D25">
+        <v>8.11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25">
+        <v>300.2</v>
+      </c>
+      <c r="I25">
+        <v>4</v>
+      </c>
+      <c r="J25">
+        <v>297.3</v>
+      </c>
+      <c r="K25">
+        <v>10.0</v>
+      </c>
+      <c r="L25" t="s">
+        <v>36</v>
+      </c>
+      <c r="M25" t="s">
+        <v>24</v>
+      </c>
+      <c r="N25" t="s">
+        <v>25</v>
+      </c>
+      <c r="O25" t="s">
+        <v>26</v>
+      </c>
+      <c r="P25" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>28</v>
+      </c>
+      <c r="R25" t="s">
+        <v>37</v>
+      </c>
+      <c r="S25" t="s">
+        <v>37</v>
+      </c>
+      <c r="T25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26">
+        <v>121.2</v>
+      </c>
+      <c r="D26">
+        <v>12.33</v>
+      </c>
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26">
+        <v>123.12</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>112.314</v>
+      </c>
+      <c r="K26">
+        <v>11.0</v>
+      </c>
+      <c r="L26" t="s">
+        <v>24</v>
+      </c>
+      <c r="M26" t="s">
+        <v>24</v>
+      </c>
+      <c r="N26" t="s">
+        <v>25</v>
+      </c>
+      <c r="O26" t="s">
+        <v>26</v>
+      </c>
+      <c r="P26" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>28</v>
+      </c>
+      <c r="R26" t="s">
+        <v>29</v>
+      </c>
+      <c r="S26" t="s">
+        <v>29</v>
+      </c>
+      <c r="T26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27">
+        <v>113.0</v>
+      </c>
+      <c r="D27">
+        <v>8.0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27">
+        <v>50.0</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27">
+        <v>45.0</v>
+      </c>
+      <c r="K27">
+        <v>10.0</v>
+      </c>
+      <c r="L27" t="s">
+        <v>24</v>
+      </c>
+      <c r="M27" t="s">
+        <v>24</v>
+      </c>
+      <c r="N27" t="s">
+        <v>25</v>
+      </c>
+      <c r="O27" t="s">
+        <v>26</v>
+      </c>
+      <c r="P27" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>28</v>
+      </c>
+      <c r="R27" t="s">
+        <v>29</v>
+      </c>
+      <c r="S27" t="s">
+        <v>29</v>
+      </c>
+      <c r="T27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28">
+        <v>113.567</v>
+      </c>
+      <c r="D28">
+        <v>8.768</v>
+      </c>
+      <c r="E28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" t="s">
+        <v>23</v>
+      </c>
+      <c r="H28">
+        <v>129.2</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+      <c r="J28">
+        <v>110.2</v>
+      </c>
+      <c r="K28">
+        <v>10.66</v>
+      </c>
+      <c r="L28" t="s">
+        <v>24</v>
+      </c>
+      <c r="M28" t="s">
+        <v>24</v>
+      </c>
+      <c r="N28" t="s">
+        <v>25</v>
+      </c>
+      <c r="O28" t="s">
+        <v>26</v>
+      </c>
+      <c r="P28" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>28</v>
+      </c>
+      <c r="R28" t="s">
+        <v>29</v>
+      </c>
+      <c r="S28" t="s">
+        <v>29</v>
+      </c>
+      <c r="T28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29">
+        <v>121.13</v>
+      </c>
+      <c r="D29">
+        <v>11.2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29">
+        <v>312.1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>12.3</v>
+      </c>
+      <c r="K29">
+        <v>12.0</v>
+      </c>
+      <c r="L29" t="s">
+        <v>24</v>
+      </c>
+      <c r="M29" t="s">
+        <v>24</v>
+      </c>
+      <c r="N29" t="s">
+        <v>25</v>
+      </c>
+      <c r="O29" t="s">
+        <v>26</v>
+      </c>
+      <c r="P29" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>28</v>
+      </c>
+      <c r="R29" t="s">
+        <v>29</v>
+      </c>
+      <c r="S29" t="s">
+        <v>29</v>
+      </c>
+      <c r="T29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30">
+        <v>1.0</v>
+      </c>
+      <c r="D30">
+        <v>1.0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30">
+        <v>1.0</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1.0</v>
+      </c>
+      <c r="K30">
+        <v>1.0</v>
+      </c>
+      <c r="L30" t="s">
+        <v>24</v>
+      </c>
+      <c r="M30" t="s">
+        <v>24</v>
+      </c>
+      <c r="N30" t="s">
+        <v>25</v>
+      </c>
+      <c r="O30" t="s">
+        <v>26</v>
+      </c>
+      <c r="P30" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>28</v>
+      </c>
+      <c r="R30" t="s">
+        <v>29</v>
+      </c>
+      <c r="S30" t="s">
+        <v>29</v>
+      </c>
+      <c r="T30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31">
+        <v>1.0</v>
+      </c>
+      <c r="D31">
+        <v>1.0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31">
+        <v>1.0</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>1.0</v>
+      </c>
+      <c r="K31">
+        <v>1.0</v>
+      </c>
+      <c r="L31" t="s">
+        <v>24</v>
+      </c>
+      <c r="M31" t="s">
+        <v>24</v>
+      </c>
+      <c r="N31" t="s">
+        <v>25</v>
+      </c>
+      <c r="O31" t="s">
+        <v>26</v>
+      </c>
+      <c r="P31" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>28</v>
+      </c>
+      <c r="R31" t="s">
+        <v>29</v>
+      </c>
+      <c r="S31" t="s">
+        <v>29</v>
+      </c>
+      <c r="T31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32">
+        <v>1.0</v>
+      </c>
+      <c r="D32">
+        <v>1.0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" t="s">
+        <v>23</v>
+      </c>
+      <c r="H32">
+        <v>1.0</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>1.0</v>
+      </c>
+      <c r="K32">
+        <v>1.0</v>
+      </c>
+      <c r="L32" t="s">
+        <v>24</v>
+      </c>
+      <c r="M32" t="s">
+        <v>24</v>
+      </c>
+      <c r="N32" t="s">
+        <v>25</v>
+      </c>
+      <c r="O32" t="s">
+        <v>26</v>
+      </c>
+      <c r="P32" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>28</v>
+      </c>
+      <c r="R32" t="s">
+        <v>29</v>
+      </c>
+      <c r="S32" t="s">
+        <v>29</v>
+      </c>
+      <c r="T32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33">
+        <v>113.22</v>
+      </c>
+      <c r="D33">
+        <v>8.11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" t="s">
+        <v>23</v>
+      </c>
+      <c r="H33">
+        <v>300.2</v>
+      </c>
+      <c r="I33">
+        <v>4</v>
+      </c>
+      <c r="J33">
+        <v>297.3</v>
+      </c>
+      <c r="K33">
+        <v>10.0</v>
+      </c>
+      <c r="L33" t="s">
+        <v>36</v>
+      </c>
+      <c r="M33" t="s">
+        <v>24</v>
+      </c>
+      <c r="N33" t="s">
+        <v>25</v>
+      </c>
+      <c r="O33" t="s">
+        <v>26</v>
+      </c>
+      <c r="P33" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>28</v>
+      </c>
+      <c r="R33" t="s">
+        <v>37</v>
+      </c>
+      <c r="S33" t="s">
+        <v>37</v>
+      </c>
+      <c r="T33" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
menambah nomer pada gedung, kerusakan
</commit_message>
<xml_diff>
--- a/public/master_gedung.xlsx
+++ b/public/master_gedung.xlsx
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
+  <si>
+    <t>No.</t>
+  </si>
   <si>
     <t>Nama</t>
   </si>
@@ -87,6 +90,81 @@
   </si>
   <si>
     <t>RTH</t>
+  </si>
+  <si>
+    <t>SMA Negeri 3 Surabaya</t>
+  </si>
+  <si>
+    <t>Jl. Memet Sastrowiryo No.54, Komp. Kenjeran, Kec. Bulak, Kota Surabaya, Jawa Timur 60121</t>
+  </si>
+  <si>
+    <t>Legal</t>
+  </si>
+  <si>
+    <t>Negara</t>
+  </si>
+  <si>
+    <t>Letter C</t>
+  </si>
+  <si>
+    <t>Kompleksitas Sedang</t>
+  </si>
+  <si>
+    <t>Lokasi Kepadatan Sedang</t>
+  </si>
+  <si>
+    <t>Permanen</t>
+  </si>
+  <si>
+    <t>Rendah</t>
+  </si>
+  <si>
+    <t>Pasif</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>SMA Negeri 1 Tuban</t>
+  </si>
+  <si>
+    <t>Jl. WR Supratman No.2, Sendang Harjo, Sendangharjo, Kec. Tuban, Kabupaten Tuban, Jawa Timur 62319</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>SMA Negeri 2 Tuban</t>
+  </si>
+  <si>
+    <t>Jl. DR. Wahidin Sudirohusodo No.867, Sidorejo, Kec. Tuban, Kabupaten Tuban, Jawa Timur 62315</t>
+  </si>
+  <si>
+    <t>Rumah Sakit Dr. R. Koesma</t>
+  </si>
+  <si>
+    <t>Jl. DR. Wahidin Sudirohusodo No.800, Sidorejo, Kec. Tuban, Kabupaten Tuban, Jawa Timur 62315</t>
+  </si>
+  <si>
+    <t>Polres Tuban</t>
+  </si>
+  <si>
+    <t>Jalan Dokter Wahidin SH, Sidorejo, Kec. Tuban, Kabupaten Tuban, Jawa Timur 62313</t>
   </si>
 </sst>
 </file>
@@ -440,7 +518,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="L7" sqref="L7"/>
@@ -466,80 +544,465 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" customHeight="1" ht="30">
-      <c r="A1" s="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>113.0</v>
+      </c>
+      <c r="E2">
+        <v>8.0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2">
+        <v>210.1</v>
+      </c>
+      <c r="J2">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="K2">
+        <v>40.12</v>
+      </c>
+      <c r="L2">
+        <v>3.12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2" t="s">
+        <v>35</v>
+      </c>
+      <c r="V2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3">
+        <v>112.0</v>
+      </c>
+      <c r="E3">
+        <v>8.0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3">
+        <v>120.231</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>20.12</v>
+      </c>
+      <c r="L3">
+        <v>21.0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V3" t="s">
+        <v>43</v>
+      </c>
+      <c r="W3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4">
+        <v>112.0</v>
+      </c>
+      <c r="E4">
+        <v>7.0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4">
+        <v>231.0</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>20.12</v>
+      </c>
+      <c r="L4">
+        <v>2.0</v>
+      </c>
+      <c r="M4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" t="s">
+        <v>36</v>
+      </c>
+      <c r="T4" t="s">
+        <v>35</v>
+      </c>
+      <c r="U4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V4" t="s">
+        <v>43</v>
+      </c>
+      <c r="W4" t="s">
+        <v>37</v>
+      </c>
+      <c r="X4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5">
+        <v>111.0</v>
+      </c>
+      <c r="E5">
+        <v>9.0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5">
+        <v>231.0</v>
+      </c>
+      <c r="J5">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>23</v>
+      <c r="K5">
+        <v>12.0</v>
+      </c>
+      <c r="L5">
+        <v>21.0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V5" t="s">
+        <v>43</v>
+      </c>
+      <c r="W5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6">
+        <v>112.0</v>
+      </c>
+      <c r="E6">
+        <v>8.0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6">
+        <v>231.0</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>12.0</v>
+      </c>
+      <c r="L6">
+        <v>21.0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R6" t="s">
+        <v>35</v>
+      </c>
+      <c r="S6" t="s">
+        <v>36</v>
+      </c>
+      <c r="T6" t="s">
+        <v>35</v>
+      </c>
+      <c r="U6" t="s">
+        <v>35</v>
+      </c>
+      <c r="V6" t="s">
+        <v>43</v>
+      </c>
+      <c r="W6" t="s">
+        <v>37</v>
+      </c>
+      <c r="X6" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>